<commit_message>
description - increased versioning and localization document Bug - TA22441 Reviewer - Deepthi Comments - NA
</commit_message>
<xml_diff>
--- a/hor-productregistration-localization/Localization.xlsx
+++ b/hor-productregistration-localization/Localization.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\310201263\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PR\hor-productregistration-android\hor-productregistration-localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Localization!$A$1:$BC$6</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2603" uniqueCount="2353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2625" uniqueCount="2375">
   <si>
     <t>Reference</t>
   </si>
@@ -25041,12 +25041,78 @@
   </si>
   <si>
     <t>tr</t>
+  </si>
+  <si>
+    <t>PPR_Find_Serial_Number</t>
+  </si>
+  <si>
+    <t>Where can I find my serial number?</t>
+  </si>
+  <si>
+    <t>PPR_find_serial_number_help_message</t>
+  </si>
+  <si>
+    <t>Engraved on the back of the product, in the compartment under the plastic cover, under the trimmer or under the shaving head</t>
+  </si>
+  <si>
+    <t>PPR_ok_i_found_it</t>
+  </si>
+  <si>
+    <t>OK, I found it</t>
+  </si>
+  <si>
+    <t>PPR_registered</t>
+  </si>
+  <si>
+    <t>Registered</t>
+  </si>
+  <si>
+    <t>PPR_registered_on</t>
+  </si>
+  <si>
+    <t>Registered on</t>
+  </si>
+  <si>
+    <t>PPR_warranty_until</t>
+  </si>
+  <si>
+    <t>Warranty until</t>
+  </si>
+  <si>
+    <t>PPR_registered_serial</t>
+  </si>
+  <si>
+    <t>You have registered serial</t>
+  </si>
+  <si>
+    <t>PPR_before</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>PPR_serial_number_consists</t>
+  </si>
+  <si>
+    <t>The serial number consists of</t>
+  </si>
+  <si>
+    <t>PPR_number_starting</t>
+  </si>
+  <si>
+    <t>PPR_eg</t>
+  </si>
+  <si>
+    <t>numbers, starting with</t>
+  </si>
+  <si>
+    <t>.E.g.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -30815,24 +30881,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IW50"/>
+  <dimension ref="A1:IW61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.3984375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="39.3828125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="92.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.3828125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.61328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.3828125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.61328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="92.921875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="55" width="65" style="1" customWidth="1"/>
-    <col min="56" max="257" width="39.3984375" style="1" customWidth="1"/>
+    <col min="56" max="257" width="39.3828125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:60" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -31004,7 +31070,7 @@
       <c r="BG1" s="10"/>
       <c r="BH1" s="11"/>
     </row>
-    <row r="2" spans="1:60" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="4" t="s">
@@ -31170,7 +31236,7 @@
       <c r="BG2" s="12"/>
       <c r="BH2" s="13"/>
     </row>
-    <row r="3" spans="1:60" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:60" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="4" t="s">
@@ -31338,7 +31404,7 @@
       <c r="BG3" s="2"/>
       <c r="BH3" s="3"/>
     </row>
-    <row r="4" spans="1:60" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:60" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="4" t="s">
@@ -31504,7 +31570,7 @@
       <c r="BG4" s="2"/>
       <c r="BH4" s="3"/>
     </row>
-    <row r="5" spans="1:60" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:60" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="4" t="s">
@@ -31670,7 +31736,7 @@
       <c r="BG5" s="2"/>
       <c r="BH5" s="3"/>
     </row>
-    <row r="6" spans="1:60" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:60" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="4" t="s">
@@ -31838,7 +31904,7 @@
       <c r="BG6" s="2"/>
       <c r="BH6" s="3"/>
     </row>
-    <row r="7" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="4" t="s">
@@ -32001,7 +32067,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="8" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="4" t="s">
@@ -32162,7 +32228,7 @@
         <v>1626</v>
       </c>
     </row>
-    <row r="9" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="4" t="s">
@@ -32323,7 +32389,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="10" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="4" t="s">
@@ -32484,7 +32550,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="11" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="4" t="s">
@@ -32645,7 +32711,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="12" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="4" t="s">
@@ -32808,7 +32874,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="13" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="4" t="s">
@@ -32971,7 +33037,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="14" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="4" t="s">
@@ -33132,7 +33198,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="15" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="4" t="s">
@@ -33293,7 +33359,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="16" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="4" t="s">
@@ -33454,7 +33520,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="17" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="4" t="s">
@@ -33615,7 +33681,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="18" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="4" t="s">
@@ -33776,7 +33842,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="19" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="4" t="s">
@@ -33937,7 +34003,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="20" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="4" t="s">
@@ -34098,7 +34164,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="21" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="4" t="s">
@@ -34259,7 +34325,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="22" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="4" t="s">
@@ -34420,7 +34486,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="23" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="4" t="s">
@@ -34581,7 +34647,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="24" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="4" t="s">
@@ -34742,7 +34808,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="25" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="4" t="s">
@@ -34903,7 +34969,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="26" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="4" t="s">
@@ -35064,7 +35130,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="27" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="4" t="s">
@@ -35225,7 +35291,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="28" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="4" t="s">
@@ -35386,7 +35452,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="29" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="4" t="s">
@@ -35547,7 +35613,7 @@
         <v>1646</v>
       </c>
     </row>
-    <row r="30" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="4" t="s">
@@ -35708,7 +35774,7 @@
         <v>1647</v>
       </c>
     </row>
-    <row r="31" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="19" t="s">
@@ -35869,7 +35935,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="32" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="19" t="s">
@@ -36030,7 +36096,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="33" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:55" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="4" t="s">
@@ -36191,7 +36257,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="34" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="4" t="s">
@@ -36352,7 +36418,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="35" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="4" t="s">
@@ -36513,7 +36579,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="36" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15"/>
       <c r="B36" s="16"/>
       <c r="C36" s="17" t="s">
@@ -36674,7 +36740,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="37" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15"/>
       <c r="B37" s="16"/>
       <c r="C37" s="20" t="s">
@@ -36837,7 +36903,7 @@
         <v>1654</v>
       </c>
     </row>
-    <row r="38" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
       <c r="B38" s="16"/>
       <c r="C38" s="17" t="s">
@@ -36998,7 +37064,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="39" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15"/>
       <c r="B39" s="16"/>
       <c r="C39" s="17" t="s">
@@ -37159,7 +37225,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="40" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15"/>
       <c r="B40" s="16"/>
       <c r="C40" s="17" t="s">
@@ -37320,7 +37386,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="41" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15"/>
       <c r="B41" s="16"/>
       <c r="C41" s="17" t="s">
@@ -37481,7 +37547,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="42" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
       <c r="B42" s="16"/>
       <c r="C42" s="17" t="s">
@@ -37642,7 +37708,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="43" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4" t="s">
@@ -37803,7 +37869,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="44" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
@@ -37964,7 +38030,7 @@
         <v>1659</v>
       </c>
     </row>
-    <row r="45" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4" t="s">
@@ -38125,7 +38191,7 @@
         <v>2273</v>
       </c>
     </row>
-    <row r="46" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="23"/>
       <c r="B46" s="23"/>
       <c r="C46" s="4" t="s">
@@ -38286,7 +38352,7 @@
         <v>2274</v>
       </c>
     </row>
-    <row r="47" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C47" s="4" t="s">
         <v>2052</v>
       </c>
@@ -38445,7 +38511,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="48" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C48" s="4" t="s">
         <v>2054</v>
       </c>
@@ -38604,7 +38670,7 @@
         <v>2276</v>
       </c>
     </row>
-    <row r="49" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="4" t="s">
         <v>2056</v>
       </c>
@@ -38763,7 +38829,7 @@
         <v>2277</v>
       </c>
     </row>
-    <row r="50" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="4" t="s">
         <v>2058</v>
       </c>
@@ -38920,6 +38986,105 @@
       </c>
       <c r="BC50" s="4" t="s">
         <v>2077</v>
+      </c>
+    </row>
+    <row r="51" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="17" t="s">
+        <v>2353</v>
+      </c>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17" t="s">
+        <v>2354</v>
+      </c>
+    </row>
+    <row r="52" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="17" t="s">
+        <v>2355</v>
+      </c>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17" t="s">
+        <v>2356</v>
+      </c>
+    </row>
+    <row r="53" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="17" t="s">
+        <v>2357</v>
+      </c>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17" t="s">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="54" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="17" t="s">
+        <v>2359</v>
+      </c>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17" t="s">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="55" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="17" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17" t="s">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="56" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="17" t="s">
+        <v>2363</v>
+      </c>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17" t="s">
+        <v>2364</v>
+      </c>
+    </row>
+    <row r="57" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="17" t="s">
+        <v>2365</v>
+      </c>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17" t="s">
+        <v>2366</v>
+      </c>
+    </row>
+    <row r="58" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="17" t="s">
+        <v>2367</v>
+      </c>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17" t="s">
+        <v>2368</v>
+      </c>
+    </row>
+    <row r="59" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="17" t="s">
+        <v>2369</v>
+      </c>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17" t="s">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="60" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="17" t="s">
+        <v>2371</v>
+      </c>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17" t="s">
+        <v>2373</v>
+      </c>
+    </row>
+    <row r="61" spans="3:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="17" t="s">
+        <v>2372</v>
+      </c>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17" t="s">
+        <v>2374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>